<commit_message>
add glob finder and baseCommand check
</commit_message>
<xml_diff>
--- a/src/ISA-CWL-Converter/data/isa.assay.neu.xlsx
+++ b/src/ISA-CWL-Converter/data/isa.assay.neu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Dataplant\IsaToCwl\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\source\repos\ISA-CWL-Converter\src\ISA-CWL-Converter\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4356D25C-58F7-4809-91F8-5C20FB02A1CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646DA8D9-A53D-4C9C-96A6-701347BEB048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t>Source Name</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>Comment[&lt;Worksheet&gt;]</t>
+  </si>
+  <si>
+    <t>hello2.txt</t>
+  </si>
+  <si>
+    <t>hello2.tar</t>
   </si>
 </sst>
 </file>
@@ -194,7 +200,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -238,8 +244,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5ABA4149-4370-43FE-9BE1-4E3DE831AE32}" name="annotationTableEmptyInsect78" displayName="annotationTableEmptyInsect78" ref="A1:K2" totalsRowShown="0">
-  <autoFilter ref="A1:K2" xr:uid="{5ABA4149-4370-43FE-9BE1-4E3DE831AE32}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5ABA4149-4370-43FE-9BE1-4E3DE831AE32}" name="annotationTableEmptyInsect78" displayName="annotationTableEmptyInsect78" ref="A1:K3" totalsRowShown="0">
+  <autoFilter ref="A1:K3" xr:uid="{5ABA4149-4370-43FE-9BE1-4E3DE831AE32}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{0C847BB6-5067-4C6B-970F-2A46F6750895}" name="Source Name"/>
     <tableColumn id="6" xr3:uid="{11DDBDA0-1331-437A-9508-C0786B115FF2}" name="Characteristic [Position]" dataDxfId="8"/>
@@ -551,27 +557,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="24.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.86328125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="29" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.59765625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="0" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="29.1328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.86328125" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="29" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -606,7 +612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -621,6 +627,23 @@
       </c>
       <c r="K2" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -635,18 +658,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3F9FB5-416C-44CF-82BC-AACA0858391C}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -654,7 +677,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -662,7 +685,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -670,7 +693,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -678,7 +701,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -686,7 +709,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -694,7 +717,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -702,7 +725,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -710,12 +733,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -723,7 +746,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -731,7 +754,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -739,7 +762,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -747,7 +770,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -755,7 +778,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -763,7 +786,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -771,7 +794,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -779,7 +802,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -787,7 +810,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -795,7 +818,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -803,7 +826,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>38</v>
       </c>

</xml_diff>